<commit_message>
change worker menu, and get_sales_report
</commit_message>
<xml_diff>
--- a/final project/Constraints1.xlsx
+++ b/final project/Constraints1.xlsx
@@ -8,21 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="shifts" sheetId="1" r:id="rId1"/>
-    <sheet name="stav" sheetId="2" r:id="rId2"/>
-    <sheet name="tair" sheetId="3" r:id="rId3"/>
-    <sheet name="yoni" sheetId="4" r:id="rId4"/>
-    <sheet name="asaf" sheetId="5" r:id="rId5"/>
-    <sheet name="rotem" sheetId="6" r:id="rId6"/>
-    <sheet name="michal" sheetId="7" r:id="rId7"/>
-    <sheet name="emilia" sheetId="8" r:id="rId8"/>
-    <sheet name="adir" sheetId="9" r:id="rId9"/>
+    <sheet name="yoni" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
   <si>
     <t>Sunday</t>
   </si>
@@ -614,6 +607,9 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
       <c r="G2" t="s">
         <v>17</v>
       </c>
@@ -621,382 +617,6 @@
     <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added check for correct input in add_worker_Constraints
</commit_message>
<xml_diff>
--- a/final project/Constraints1.xlsx
+++ b/final project/Constraints1.xlsx
@@ -9,13 +9,15 @@
   <sheets>
     <sheet name="shifts" sheetId="1" r:id="rId1"/>
     <sheet name="yoni" sheetId="2" r:id="rId2"/>
+    <sheet name="tair" sheetId="3" r:id="rId3"/>
+    <sheet name="asaf" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="18">
   <si>
     <t>Sunday</t>
   </si>
@@ -622,4 +624,108 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
almost_final_project.py- the file that runs the project project_for_test.py- the file for unit test
</commit_message>
<xml_diff>
--- a/final project/Constraints1.xlsx
+++ b/final project/Constraints1.xlsx
@@ -8,16 +8,21 @@
   </bookViews>
   <sheets>
     <sheet name="shifts" sheetId="1" r:id="rId1"/>
-    <sheet name="yoni" sheetId="2" r:id="rId2"/>
-    <sheet name="tair" sheetId="3" r:id="rId3"/>
-    <sheet name="asaf" sheetId="4" r:id="rId4"/>
+    <sheet name="tair" sheetId="2" r:id="rId2"/>
+    <sheet name="asaf" sheetId="3" r:id="rId3"/>
+    <sheet name="yoni" sheetId="4" r:id="rId4"/>
+    <sheet name="adir" sheetId="5" r:id="rId5"/>
+    <sheet name="stav" sheetId="6" r:id="rId6"/>
+    <sheet name="rotem" sheetId="7" r:id="rId7"/>
+    <sheet name="michal" sheetId="8" r:id="rId8"/>
+    <sheet name="emilia" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="19">
   <si>
     <t>Sunday</t>
   </si>
@@ -43,31 +48,34 @@
     <t>Morning</t>
   </si>
   <si>
+    <t>rotem</t>
+  </si>
+  <si>
+    <t>yoni</t>
+  </si>
+  <si>
+    <t>stav</t>
+  </si>
+  <si>
+    <t>adir</t>
+  </si>
+  <si>
     <t>tair</t>
   </si>
   <si>
+    <t>shift manager</t>
+  </si>
+  <si>
+    <t>michal</t>
+  </si>
+  <si>
+    <t>emilia</t>
+  </si>
+  <si>
+    <t>Evening</t>
+  </si>
+  <si>
     <t>asaf</t>
-  </si>
-  <si>
-    <t>yoni</t>
-  </si>
-  <si>
-    <t>rotem</t>
-  </si>
-  <si>
-    <t>stav</t>
-  </si>
-  <si>
-    <t>shift manager</t>
-  </si>
-  <si>
-    <t>emilia</t>
-  </si>
-  <si>
-    <t>michal</t>
-  </si>
-  <si>
-    <t>Evening</t>
   </si>
   <si>
     <t>NO</t>
@@ -442,16 +450,16 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -459,22 +467,22 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -488,13 +496,13 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>
@@ -505,19 +513,19 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
         <v>9</v>
@@ -528,22 +536,22 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -557,13 +565,13 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
       </c>
       <c r="H7" t="s">
         <v>14</v>
@@ -609,16 +617,16 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
+      <c r="E2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -661,16 +669,16 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
+      <c r="B2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
+      <c r="C3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -713,16 +721,276 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
+      <c r="D2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add check in make changes
</commit_message>
<xml_diff>
--- a/final project/Constraints1.xlsx
+++ b/final project/Constraints1.xlsx
@@ -48,34 +48,34 @@
     <t>Morning</t>
   </si>
   <si>
+    <t>tair</t>
+  </si>
+  <si>
+    <t>adir</t>
+  </si>
+  <si>
+    <t>stav</t>
+  </si>
+  <si>
+    <t>yoni</t>
+  </si>
+  <si>
     <t>rotem</t>
   </si>
   <si>
-    <t>yoni</t>
-  </si>
-  <si>
-    <t>stav</t>
-  </si>
-  <si>
-    <t>adir</t>
-  </si>
-  <si>
-    <t>tair</t>
+    <t>shift manager</t>
+  </si>
+  <si>
+    <t>michal</t>
+  </si>
+  <si>
+    <t>emilia</t>
+  </si>
+  <si>
+    <t>Evening</t>
   </si>
   <si>
     <t>asaf</t>
-  </si>
-  <si>
-    <t>shift manager</t>
-  </si>
-  <si>
-    <t>michal</t>
-  </si>
-  <si>
-    <t>emilia</t>
-  </si>
-  <si>
-    <t>Evening</t>
   </si>
   <si>
     <t>NO</t>
@@ -456,10 +456,10 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -467,65 +467,65 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
       <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
       <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
         <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
       </c>
       <c r="H5" t="s">
         <v>9</v>
@@ -533,48 +533,48 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
       <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
         <v>15</v>
       </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -623,7 +623,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>
@@ -669,15 +669,15 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -727,9 +727,9 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -779,9 +779,9 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -825,13 +825,13 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
       </c>
       <c r="H3" t="s">
         <v>18</v>
@@ -877,13 +877,13 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
       </c>
       <c r="H3" t="s">
         <v>18</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
         <v>18</v>
@@ -987,7 +987,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>

</xml_diff>